<commit_message>
Updated the miscellanous folder
</commit_message>
<xml_diff>
--- a/Phase_I/End-Sem_Aeroplane/85thresh_80epoch/updated_annotations/test_results.xlsx
+++ b/Phase_I/End-Sem_Aeroplane/85thresh_80epoch/updated_annotations/test_results.xlsx
@@ -57,12 +57,12 @@
     <t>007654</t>
   </si>
   <si>
+    <t>007677</t>
+  </si>
+  <si>
     <t>STOP q-value</t>
   </si>
   <si>
-    <t>007677</t>
-  </si>
-  <si>
     <t>007723</t>
   </si>
   <si>
@@ -150,7 +150,7 @@
     <t>IoU decrease: 8</t>
   </si>
   <si>
-    <t>IoU average: 0.5623925279971539</t>
+    <t>IoU average: 0.5635587432643805</t>
   </si>
 </sst>
 </file>
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,13 +570,13 @@
         <v>7</v>
       </c>
       <c r="J2">
+        <v>0.63</v>
+      </c>
+      <c r="K2">
         <v>0.53</v>
       </c>
-      <c r="K2">
-        <v>0.49</v>
-      </c>
       <c r="L2">
-        <v>0.53</v>
+        <v>0.63</v>
       </c>
       <c r="M2">
         <v>10</v>
@@ -614,27 +614,27 @@
         <v>11</v>
       </c>
       <c r="J3">
+        <v>0.34</v>
+      </c>
+      <c r="K3">
         <v>0.21</v>
       </c>
-      <c r="K3">
-        <v>0.18</v>
-      </c>
       <c r="L3">
-        <v>0.21</v>
+        <v>0.34</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>0.52</v>
@@ -652,19 +652,19 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4">
+        <v>0.15</v>
+      </c>
+      <c r="K4">
         <v>0.11</v>
       </c>
-      <c r="K4">
-        <v>0.09</v>
-      </c>
       <c r="L4">
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="M4">
         <v>10</v>
@@ -699,60 +699,60 @@
         <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J5">
-        <v>0.15</v>
+        <v>0.47</v>
       </c>
       <c r="K5">
-        <v>0.12</v>
+        <v>0.45</v>
       </c>
       <c r="L5">
-        <v>0.15</v>
+        <v>0.47</v>
       </c>
       <c r="M5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>0.45</v>
+        <v>0.33</v>
       </c>
       <c r="C6">
-        <v>0.49</v>
+        <v>0.53</v>
       </c>
       <c r="D6">
-        <v>0.49</v>
+        <v>0.53</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
       </c>
       <c r="J6">
+        <v>0.86</v>
+      </c>
+      <c r="K6">
         <v>0.83</v>
       </c>
-      <c r="K6">
-        <v>0.8</v>
-      </c>
       <c r="L6">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="M6">
         <v>10</v>
@@ -790,22 +790,22 @@
         <v>30</v>
       </c>
       <c r="J7">
+        <v>0.91</v>
+      </c>
+      <c r="K7">
         <v>0.78</v>
       </c>
-      <c r="K7">
-        <v>0.64</v>
-      </c>
       <c r="L7">
-        <v>0.78</v>
+        <v>0.91</v>
       </c>
       <c r="M7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -834,22 +834,22 @@
         <v>31</v>
       </c>
       <c r="J8">
+        <v>0.71</v>
+      </c>
+      <c r="K8">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K8">
-        <v>0.39</v>
-      </c>
       <c r="L8">
-        <v>0.55000000000000004</v>
+        <v>0.71</v>
       </c>
       <c r="M8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -878,22 +878,22 @@
         <v>32</v>
       </c>
       <c r="J9">
+        <v>0.46</v>
+      </c>
+      <c r="K9">
         <v>0.43</v>
       </c>
-      <c r="K9">
-        <v>0.42</v>
-      </c>
       <c r="L9">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -962,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -993,7 +993,7 @@
         <v>25</v>
       </c>
       <c r="B14">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
       <c r="C14">
         <v>0.55000000000000004</v>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1132,15 +1132,15 @@
       </c>
       <c r="C20">
         <f>AVERAGE(C2:C19)</f>
-        <v>0.59555555555555562</v>
+        <v>0.59777777777777785</v>
       </c>
       <c r="D20">
         <f>AVERAGE(D2:D19)</f>
-        <v>0.61888888888888882</v>
+        <v>0.62111111111111117</v>
       </c>
       <c r="E20">
         <f>AVERAGE(E2:E19)</f>
-        <v>8.2222222222222214</v>
+        <v>8.6111111111111107</v>
       </c>
       <c r="F20">
         <f>AVERAGE(F2:F19)</f>
@@ -1151,15 +1151,15 @@
       </c>
       <c r="K20">
         <f>AVERAGE(K2:K9)</f>
-        <v>0.39124999999999999</v>
+        <v>0.48625000000000002</v>
       </c>
       <c r="L20">
         <f>AVERAGE(L2:L9)</f>
-        <v>0.45624999999999999</v>
+        <v>0.5675</v>
       </c>
       <c r="M20">
         <f>AVERAGE(M2:M9)</f>
-        <v>7.5</v>
+        <v>7.125</v>
       </c>
       <c r="N20">
         <f>AVERAGE(N2:N9)</f>
@@ -1185,13 +1185,13 @@
         <v>36</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I23" t="s">
         <v>40</v>
       </c>
       <c r="J23">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -1214,28 +1214,28 @@
       </c>
       <c r="B25">
         <f>(SUM(C2:C19)-SUM(B2:B19))/18</f>
-        <v>6.1111111111111088E-2</v>
+        <v>7.0555555555555538E-2</v>
       </c>
       <c r="I25" t="s">
         <v>38</v>
       </c>
       <c r="J25">
         <f>(SUM(K2:K9)-SUM(J2:J9))/8</f>
-        <v>-5.7500000000000051E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>41</v>
+        <v>-8.0000000000000016E-2</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>